<commit_message>
Fixed a bug that caused the study guide module to be deleted if the modules were also scaffolded; Fixed a bug that depended on assignments and quizes to be scaffolded at the same time as module items; Added configs for all Frontend frameworks courses
</commit_message>
<xml_diff>
--- a/frontend-frameworks-zb0151/config.xlsx
+++ b/frontend-frameworks-zb0151/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\canvas-course-scaffolder-with-course-configs\frontend-frameworks-zb0151\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1B1A2F-3F65-43F5-9D03-90117B4839CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BBCF4A-3182-40BC-BE7F-F8C896A304E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemene info" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="121">
   <si>
     <t>Naam</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Permanente Evaluatie</t>
   </si>
   <si>
-    <t>Upload Permanente Evaluatie</t>
-  </si>
-  <si>
     <t>Les 1 - Componenten</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>Opgave</t>
   </si>
   <si>
-    <t>Oplossing</t>
-  </si>
-  <si>
     <t>https://gitpub.sebastiaanh.com/public/web/b7b82925-1ec6-4862-bb61-9e050f4d9807/</t>
   </si>
   <si>
@@ -364,6 +358,57 @@
   </si>
   <si>
     <t>QUIZ</t>
+  </si>
+  <si>
+    <t>Oplossing (Code)</t>
+  </si>
+  <si>
+    <t>Oplossing (Video)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PL_YNuJASOTQK8iJ7ODt7V9_8Nf1aE8LJt</t>
+  </si>
+  <si>
+    <t>Algemene informatie</t>
+  </si>
+  <si>
+    <t>Cursusmateriaal</t>
+  </si>
+  <si>
+    <t>Cursuswebsite</t>
+  </si>
+  <si>
+    <t>Cursusmateriaal (Offline installer)</t>
+  </si>
+  <si>
+    <t>https://github.com/it-graduaten/Releases-JavaScript-Leerlijn/releases</t>
+  </si>
+  <si>
+    <t>Teams vergaderingen</t>
+  </si>
+  <si>
+    <t>https://teams.microsoft.com/l/meetup-join/19%3ameeting_YWNiMGU3ZGMtZjFkNS00YTQ1LThiZmQtYmJmMjQzNzFmOWQ2%40thread.v2/0?context=%7b%22Tid%22%3a%2277d33cc5-c9b4-4766-95c7-ed5b515e1cce%22%2c%22Oid%22%3a%2293730d70-def5-4b40-a5ff-060158ac12ec%22%7d</t>
+  </si>
+  <si>
+    <t>https://teams.microsoft.com/l/meetup-join/19%3ameeting_MmJhMGZhMmEtOGQ3Ny00ZDBmLWE2YmYtZGMzMGQ5MzAzOTI0%40thread.v2/0?context=%7b%22Tid%22%3a%2277d33cc5-c9b4-4766-95c7-ed5b515e1cce%22%2c%22Oid%22%3a%2293730d70-def5-4b40-a5ff-060158ac12ec%22%7d</t>
+  </si>
+  <si>
+    <t>Online Lessen: Geel</t>
+  </si>
+  <si>
+    <t>Online Lessen: Turnhout</t>
+  </si>
+  <si>
+    <t>Online Lessen: Lier</t>
+  </si>
+  <si>
+    <t>https://teams.microsoft.com/l/meetup-join/19%3ameeting_MDdiYmE1NjEtMWFhOS00ZWZmLTk5YmMtYWM0OWVhN2ExMmZj%40thread.v2/0?context=%7b%22Tid%22%3a%2277d33cc5-c9b4-4766-95c7-ed5b515e1cce%22%2c%22Oid%22%3a%2293730d70-def5-4b40-a5ff-060158ac12ec%22%7d</t>
+  </si>
+  <si>
+    <t>GitHub Classroom Assignment</t>
+  </si>
+  <si>
+    <t>https://classroom.github.com/a/n2HSrcQF</t>
   </si>
 </sst>
 </file>
@@ -435,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -529,8 +574,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}" name="Tabel3567" displayName="Tabel3567" ref="A1:I62" totalsRowShown="0">
-  <autoFilter ref="A1:I62" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}" name="Tabel3567" displayName="Tabel3567" ref="A1:I73" totalsRowShown="0">
+  <autoFilter ref="A1:I73" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F1B940E-7EAD-48A5-AA1E-A5E5ED525C5C}" name="Module"/>
     <tableColumn id="2" xr3:uid="{54A84E46-41BB-4012-84B6-2A4A1FB473F4}" name="Type"/>
@@ -824,7 +869,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,7 +987,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -1135,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E457B5F6-0D60-4A35-BC13-7D2947E918FD}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,7 +1210,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1173,7 +1218,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1189,7 +1234,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1197,7 +1242,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1205,7 +1250,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1213,7 +1258,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1221,7 +1266,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1229,7 +1274,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1237,7 +1282,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1245,9 +1290,17 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13">
         <v>1</v>
       </c>
     </row>
@@ -1262,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E63DFD8-2013-40A2-8CE5-0CB5ABE5CD54}">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1307,15 +1360,15 @@
         <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1329,10 +1382,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
@@ -1352,7 +1405,7 @@
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1363,87 +1416,73 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
+      <c r="F5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
-        <v>61</v>
-      </c>
       <c r="I7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>55</v>
+      <c r="F9" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1451,911 +1490,1102 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="I10">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="I13">
         <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D15">
         <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
         <v>56</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" t="s">
         <v>62</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="P38" s="3"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="s">
         <v>52</v>
       </c>
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
         <v>59</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18">
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I48">
         <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>74</v>
-      </c>
-      <c r="I19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="P30" s="3"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" t="s">
-        <v>59</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I48">
-        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C49" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D49">
         <v>1</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I49">
-        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I51">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I53">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D54">
         <v>1</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I54">
-        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" t="s">
         <v>52</v>
       </c>
-      <c r="C55" t="s">
-        <v>60</v>
-      </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D56">
         <v>1</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I56">
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I58">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" t="s">
+        <v>62</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C60" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="I60">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B61" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" t="s">
         <v>52</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>50</v>
+      </c>
+      <c r="B66" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" t="s">
         <v>59</v>
       </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>82</v>
-      </c>
-      <c r="B62" t="s">
-        <v>52</v>
-      </c>
-      <c r="C62" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62">
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>50</v>
+      </c>
+      <c r="B67" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67" t="s">
+        <v>61</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>50</v>
+      </c>
+      <c r="B68" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" t="s">
+        <v>62</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" t="s">
+        <v>104</v>
+      </c>
+      <c r="D69">
         <v>0</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="I62">
+      <c r="F69" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" t="s">
+        <v>58</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I73">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4 A6:A10 A12:A19 A21:A28 A34:A41 A43:A50 A52:A58 A60:A1048576 A30:A32" xr:uid="{05490883-A9D0-4075-B059-A05DB8772F28}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A6 A16:A21 A23:A30 A32:A39 A45:A52 A54:A61 A63:A69 A41:A43 A71:A1048576" xr:uid="{05490883-A9D0-4075-B059-A05DB8772F28}">
       <formula1>Modules</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1" xr:uid="{CD472F28-4056-4C06-A226-829362E27483}"/>
-    <hyperlink ref="F14" r:id="rId2" xr:uid="{1AEC503C-F528-46A5-8D52-204F45E67E63}"/>
-    <hyperlink ref="F15" r:id="rId3" xr:uid="{E88929C8-1B86-4617-AF62-C04E55BD4E0B}"/>
-    <hyperlink ref="F17" r:id="rId4" xr:uid="{B435E85A-25D2-4CD2-92AC-32F1D5ED8751}"/>
-    <hyperlink ref="F22" r:id="rId5" xr:uid="{CE78F98F-7BD2-4EA8-8E67-FCDB77095A12}"/>
-    <hyperlink ref="F23" r:id="rId6" xr:uid="{7DE1F5AC-CC25-429F-A3FC-D507F2EEFB16}"/>
-    <hyperlink ref="F24" r:id="rId7" xr:uid="{E87E436B-A6CF-4293-ACBA-926DFF90FF9C}"/>
-    <hyperlink ref="F26" r:id="rId8" xr:uid="{CD514174-386C-457E-9805-615309DAE21A}"/>
-    <hyperlink ref="F27" r:id="rId9" xr:uid="{01C1FF2F-6262-4AA7-93EE-58639F5D61F0}"/>
-    <hyperlink ref="F28" r:id="rId10" xr:uid="{FB0EA1FA-ADC3-44E4-B571-1621140B470F}"/>
-    <hyperlink ref="F60" r:id="rId11" xr:uid="{7A3ECBDB-E535-4B65-A061-9267A9292ADE}"/>
-    <hyperlink ref="F61" r:id="rId12" xr:uid="{AA0EA6C9-359B-4DD4-B29B-31E1B4E72016}"/>
-    <hyperlink ref="F62" r:id="rId13" xr:uid="{D49BC22E-FC53-46B7-A78B-126BD0FA3DB5}"/>
-    <hyperlink ref="F35" r:id="rId14" xr:uid="{12A5BFEB-A875-4840-839C-8B054790EB97}"/>
-    <hyperlink ref="F36" r:id="rId15" xr:uid="{6760ADEB-1ED9-4DF0-93F6-9E1C69CF29FC}"/>
-    <hyperlink ref="F37" r:id="rId16" xr:uid="{7D161BB2-F6E0-4B77-96F3-EA1340168215}"/>
-    <hyperlink ref="F39" r:id="rId17" xr:uid="{32D57917-AE6F-494D-AA32-E441EB6A079F}"/>
-    <hyperlink ref="F40" r:id="rId18" xr:uid="{69F1A799-B95D-4484-B410-26F335B45842}"/>
-    <hyperlink ref="F41" r:id="rId19" xr:uid="{ECFB4D30-9633-4881-B468-D46A967F3460}"/>
-    <hyperlink ref="F44" r:id="rId20" xr:uid="{5CF02266-2A6A-4740-A7F1-D248E7DBD25F}"/>
-    <hyperlink ref="F45" r:id="rId21" xr:uid="{5915C57B-C6AB-49C5-9FA1-9578CF01BFBD}"/>
-    <hyperlink ref="F46" r:id="rId22" xr:uid="{82328BD7-C9CF-4062-A9D1-4A43D38035B4}"/>
-    <hyperlink ref="F48" r:id="rId23" xr:uid="{43405383-4239-4B42-86DE-37B919FC09FB}"/>
-    <hyperlink ref="F49" r:id="rId24" xr:uid="{DE075D6C-8959-49B9-9D77-5C6332B4B8DA}"/>
-    <hyperlink ref="F50" r:id="rId25" xr:uid="{D149283C-ADF8-4B03-BD8B-877C4DC17423}"/>
-    <hyperlink ref="F53" r:id="rId26" xr:uid="{B23B3960-C96D-473E-BF89-5246C651B945}"/>
-    <hyperlink ref="F54" r:id="rId27" xr:uid="{B56C13F6-53AE-447D-A615-AE3C5BAF48F2}"/>
-    <hyperlink ref="F55" r:id="rId28" xr:uid="{1075C6DC-69D3-4549-8457-AE3BF3C4B442}"/>
-    <hyperlink ref="F57" r:id="rId29" xr:uid="{A20A0842-C85C-4F8E-B262-D7FAB59FCEDB}"/>
-    <hyperlink ref="F58" r:id="rId30" xr:uid="{E50DBCBB-6E47-4D79-A306-01F64E6926BA}"/>
-    <hyperlink ref="F30" r:id="rId31" xr:uid="{00C4D5F6-D9C6-4912-9229-CA2E64376E3A}"/>
-    <hyperlink ref="F31" r:id="rId32" xr:uid="{8D784FF9-973D-4416-AE5E-71E72B3070A6}"/>
-    <hyperlink ref="F32" r:id="rId33" xr:uid="{FFBC7B45-33D0-4A1F-9897-3C080883CE06}"/>
+    <hyperlink ref="F24" r:id="rId1" xr:uid="{CD472F28-4056-4C06-A226-829362E27483}"/>
+    <hyperlink ref="F25" r:id="rId2" xr:uid="{1AEC503C-F528-46A5-8D52-204F45E67E63}"/>
+    <hyperlink ref="F26" r:id="rId3" xr:uid="{E88929C8-1B86-4617-AF62-C04E55BD4E0B}"/>
+    <hyperlink ref="F28" r:id="rId4" xr:uid="{B435E85A-25D2-4CD2-92AC-32F1D5ED8751}"/>
+    <hyperlink ref="F33" r:id="rId5" xr:uid="{CE78F98F-7BD2-4EA8-8E67-FCDB77095A12}"/>
+    <hyperlink ref="F34" r:id="rId6" xr:uid="{7DE1F5AC-CC25-429F-A3FC-D507F2EEFB16}"/>
+    <hyperlink ref="F35" r:id="rId7" xr:uid="{E87E436B-A6CF-4293-ACBA-926DFF90FF9C}"/>
+    <hyperlink ref="F37" r:id="rId8" xr:uid="{CD514174-386C-457E-9805-615309DAE21A}"/>
+    <hyperlink ref="F38" r:id="rId9" xr:uid="{01C1FF2F-6262-4AA7-93EE-58639F5D61F0}"/>
+    <hyperlink ref="F39" r:id="rId10" xr:uid="{FB0EA1FA-ADC3-44E4-B571-1621140B470F}"/>
+    <hyperlink ref="F71" r:id="rId11" xr:uid="{7A3ECBDB-E535-4B65-A061-9267A9292ADE}"/>
+    <hyperlink ref="F72" r:id="rId12" xr:uid="{AA0EA6C9-359B-4DD4-B29B-31E1B4E72016}"/>
+    <hyperlink ref="F73" r:id="rId13" xr:uid="{D49BC22E-FC53-46B7-A78B-126BD0FA3DB5}"/>
+    <hyperlink ref="F46" r:id="rId14" xr:uid="{12A5BFEB-A875-4840-839C-8B054790EB97}"/>
+    <hyperlink ref="F47" r:id="rId15" xr:uid="{6760ADEB-1ED9-4DF0-93F6-9E1C69CF29FC}"/>
+    <hyperlink ref="F48" r:id="rId16" xr:uid="{7D161BB2-F6E0-4B77-96F3-EA1340168215}"/>
+    <hyperlink ref="F50" r:id="rId17" xr:uid="{32D57917-AE6F-494D-AA32-E441EB6A079F}"/>
+    <hyperlink ref="F51" r:id="rId18" xr:uid="{69F1A799-B95D-4484-B410-26F335B45842}"/>
+    <hyperlink ref="F52" r:id="rId19" xr:uid="{ECFB4D30-9633-4881-B468-D46A967F3460}"/>
+    <hyperlink ref="F55" r:id="rId20" xr:uid="{5CF02266-2A6A-4740-A7F1-D248E7DBD25F}"/>
+    <hyperlink ref="F56" r:id="rId21" xr:uid="{5915C57B-C6AB-49C5-9FA1-9578CF01BFBD}"/>
+    <hyperlink ref="F57" r:id="rId22" xr:uid="{82328BD7-C9CF-4062-A9D1-4A43D38035B4}"/>
+    <hyperlink ref="F59" r:id="rId23" xr:uid="{43405383-4239-4B42-86DE-37B919FC09FB}"/>
+    <hyperlink ref="F60" r:id="rId24" xr:uid="{DE075D6C-8959-49B9-9D77-5C6332B4B8DA}"/>
+    <hyperlink ref="F61" r:id="rId25" xr:uid="{D149283C-ADF8-4B03-BD8B-877C4DC17423}"/>
+    <hyperlink ref="F64" r:id="rId26" xr:uid="{B23B3960-C96D-473E-BF89-5246C651B945}"/>
+    <hyperlink ref="F65" r:id="rId27" xr:uid="{B56C13F6-53AE-447D-A615-AE3C5BAF48F2}"/>
+    <hyperlink ref="F66" r:id="rId28" xr:uid="{1075C6DC-69D3-4549-8457-AE3BF3C4B442}"/>
+    <hyperlink ref="F68" r:id="rId29" xr:uid="{A20A0842-C85C-4F8E-B262-D7FAB59FCEDB}"/>
+    <hyperlink ref="F69" r:id="rId30" xr:uid="{E50DBCBB-6E47-4D79-A306-01F64E6926BA}"/>
+    <hyperlink ref="F41" r:id="rId31" xr:uid="{00C4D5F6-D9C6-4912-9229-CA2E64376E3A}"/>
+    <hyperlink ref="F42" r:id="rId32" xr:uid="{8D784FF9-973D-4416-AE5E-71E72B3070A6}"/>
+    <hyperlink ref="F43" r:id="rId33" xr:uid="{FFBC7B45-33D0-4A1F-9897-3C080883CE06}"/>
+    <hyperlink ref="F8" r:id="rId34" xr:uid="{4D46C10E-C6D4-4B41-8B66-70D5F2FA3BE1}"/>
+    <hyperlink ref="F9" r:id="rId35" xr:uid="{BD53E090-37F9-4E13-AF78-B68973469EB5}"/>
+    <hyperlink ref="F11" r:id="rId36" xr:uid="{626FDF40-FBEC-469C-8841-8F876E6B0D93}"/>
+    <hyperlink ref="F12" r:id="rId37" xr:uid="{2084F117-6494-4417-9FDF-571020A1FF9B}"/>
+    <hyperlink ref="F13" r:id="rId38" xr:uid="{A4D43478-BE26-43E3-86DD-A63CC6920DAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
   <tableParts count="1">
-    <tablePart r:id="rId35"/>
+    <tablePart r:id="rId40"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fixed a broken link in the frontend config
</commit_message>
<xml_diff>
--- a/frontend-frameworks-zb0151/config.xlsx
+++ b/frontend-frameworks-zb0151/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\canvas-course-scaffolder-with-course-configs\frontend-frameworks-zb0151\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BBCF4A-3182-40BC-BE7F-F8C896A304E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE99B16-C1BD-40AC-AAD5-373173567AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="122">
   <si>
     <t>Naam</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>https://classroom.github.com/a/n2HSrcQF</t>
+  </si>
+  <si>
+    <t>https://gitpub.sebastiaanh.com/public/web/a1c9566f-cdac-4461-81a4-445c9525f86a/</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1321,7 @@
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1667,8 +1670,8 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="F20" t="s">
-        <v>63</v>
+      <c r="F20" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -2581,11 +2584,12 @@
     <hyperlink ref="F11" r:id="rId36" xr:uid="{626FDF40-FBEC-469C-8841-8F876E6B0D93}"/>
     <hyperlink ref="F12" r:id="rId37" xr:uid="{2084F117-6494-4417-9FDF-571020A1FF9B}"/>
     <hyperlink ref="F13" r:id="rId38" xr:uid="{A4D43478-BE26-43E3-86DD-A63CC6920DAE}"/>
+    <hyperlink ref="F20" r:id="rId39" xr:uid="{8B678113-A157-4982-AA60-FA3944821DE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
   <tableParts count="1">
-    <tablePart r:id="rId40"/>
+    <tablePart r:id="rId41"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added the config files for backend frameworks
</commit_message>
<xml_diff>
--- a/frontend-frameworks-zb0151/config.xlsx
+++ b/frontend-frameworks-zb0151/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\canvas-course-scaffolder-with-course-configs\frontend-frameworks-zb0151\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE99B16-C1BD-40AC-AAD5-373173567AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03775418-2D60-4DA0-BF6C-0F25B363923E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="128">
   <si>
     <t>Naam</t>
   </si>
@@ -412,6 +412,24 @@
   </si>
   <si>
     <t>https://gitpub.sebastiaanh.com/public/web/a1c9566f-cdac-4461-81a4-445c9525f86a/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PL_YNuJASOTQJ9pJP6VFVB1nkt02lHBRvp</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PL_YNuJASOTQJPwWQTEcf0bB4laX8-Oq4H</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PL_YNuJASOTQJ20pjHzkI1-mZCBokBv1oF</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PL_YNuJASOTQJw1wgXDp7HUq-RRnFQTQ7I</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PL_YNuJASOTQIgw1L3GYP0ZyLuWbWqORFz</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PL_YNuJASOTQIt3ZGDfKi8UwyddA6sTruY</t>
   </si>
 </sst>
 </file>
@@ -577,8 +595,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}" name="Tabel3567" displayName="Tabel3567" ref="A1:I73" totalsRowShown="0">
-  <autoFilter ref="A1:I73" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}" name="Tabel3567" displayName="Tabel3567" ref="A1:I79" totalsRowShown="0">
+  <autoFilter ref="A1:I79" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F1B940E-7EAD-48A5-AA1E-A5E5ED525C5C}" name="Module"/>
     <tableColumn id="2" xr3:uid="{54A84E46-41BB-4012-84B6-2A4A1FB473F4}" name="Type"/>
@@ -1318,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E63DFD8-2013-40A2-8CE5-0CB5ABE5CD54}">
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1845,18 +1863,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
@@ -1864,18 +1888,12 @@
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I33">
         <v>1</v>
       </c>
     </row>
@@ -1887,16 +1905,16 @@
         <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -1907,13 +1925,13 @@
         <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I35">
         <v>2</v>
@@ -1924,13 +1942,19 @@
         <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D36">
         <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -1938,18 +1962,12 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I37">
         <v>1</v>
       </c>
     </row>
@@ -1961,18 +1979,17 @@
         <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I38">
-        <v>2</v>
-      </c>
-      <c r="P38" s="3"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -1982,56 +1999,57 @@
         <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I39">
         <v>2</v>
       </c>
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="I41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="I42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -2042,70 +2060,76 @@
         <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I43">
         <v>0</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I43">
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I44">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I45">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
         <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="I46">
         <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" t="s">
-        <v>51</v>
-      </c>
-      <c r="C47" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I47">
-        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -2113,19 +2137,13 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D48">
         <v>1</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I48">
-        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -2133,12 +2151,18 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I49">
         <v>1</v>
       </c>
     </row>
@@ -2150,16 +2174,16 @@
         <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2170,13 +2194,13 @@
         <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I51">
         <v>2</v>
@@ -2187,92 +2211,92 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I52">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D54">
         <v>1</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I55">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
         <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="I56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>49</v>
-      </c>
-      <c r="B57" t="s">
-        <v>51</v>
-      </c>
-      <c r="C57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I57">
         <v>2</v>
       </c>
     </row>
@@ -2284,7 +2308,7 @@
         <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -2298,13 +2322,13 @@
         <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I59">
         <v>1</v>
@@ -2318,13 +2342,13 @@
         <v>51</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I60">
         <v>2</v>
@@ -2338,67 +2362,87 @@
         <v>51</v>
       </c>
       <c r="C61" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I61">
         <v>2</v>
       </c>
     </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>49</v>
+      </c>
+      <c r="B62" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B63" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I63">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B64" t="s">
         <v>51</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I64">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B65" t="s">
         <v>51</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I65">
         <v>2</v>
@@ -2406,36 +2450,22 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B66" t="s">
         <v>51</v>
       </c>
       <c r="C66" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="I66">
         <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>50</v>
-      </c>
-      <c r="B67" t="s">
-        <v>55</v>
-      </c>
-      <c r="C67" t="s">
-        <v>61</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -2443,18 +2473,12 @@
         <v>50</v>
       </c>
       <c r="B68" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C68" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D68">
-        <v>1</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I68">
         <v>1</v>
       </c>
     </row>
@@ -2466,82 +2490,196 @@
         <v>51</v>
       </c>
       <c r="C69" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>50</v>
+      </c>
+      <c r="B70" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I70">
         <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B71" t="s">
         <v>51</v>
       </c>
       <c r="C71" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I71">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C72" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D72">
-        <v>1</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I72">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73" t="s">
+        <v>62</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>50</v>
+      </c>
+      <c r="B74" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" t="s">
+        <v>104</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>50</v>
+      </c>
+      <c r="B75" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" t="s">
+        <v>105</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>80</v>
       </c>
-      <c r="B73" t="s">
-        <v>51</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B77" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" t="s">
+        <v>62</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" t="s">
+        <v>58</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" t="s">
         <v>104</v>
       </c>
-      <c r="D73">
+      <c r="D79">
         <v>0</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I73">
+      <c r="I79">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A6 A16:A21 A23:A30 A32:A39 A45:A52 A54:A61 A63:A69 A41:A43 A71:A1048576" xr:uid="{05490883-A9D0-4075-B059-A05DB8772F28}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A6 A16:A21 A23:A31 A33:A41 A48:A56 A58:A66 A68:A75 A43:A46 A77:A1048576" xr:uid="{05490883-A9D0-4075-B059-A05DB8772F28}">
       <formula1>Modules</formula1>
     </dataValidation>
   </dataValidations>
@@ -2550,46 +2688,49 @@
     <hyperlink ref="F25" r:id="rId2" xr:uid="{1AEC503C-F528-46A5-8D52-204F45E67E63}"/>
     <hyperlink ref="F26" r:id="rId3" xr:uid="{E88929C8-1B86-4617-AF62-C04E55BD4E0B}"/>
     <hyperlink ref="F28" r:id="rId4" xr:uid="{B435E85A-25D2-4CD2-92AC-32F1D5ED8751}"/>
-    <hyperlink ref="F33" r:id="rId5" xr:uid="{CE78F98F-7BD2-4EA8-8E67-FCDB77095A12}"/>
-    <hyperlink ref="F34" r:id="rId6" xr:uid="{7DE1F5AC-CC25-429F-A3FC-D507F2EEFB16}"/>
-    <hyperlink ref="F35" r:id="rId7" xr:uid="{E87E436B-A6CF-4293-ACBA-926DFF90FF9C}"/>
-    <hyperlink ref="F37" r:id="rId8" xr:uid="{CD514174-386C-457E-9805-615309DAE21A}"/>
-    <hyperlink ref="F38" r:id="rId9" xr:uid="{01C1FF2F-6262-4AA7-93EE-58639F5D61F0}"/>
-    <hyperlink ref="F39" r:id="rId10" xr:uid="{FB0EA1FA-ADC3-44E4-B571-1621140B470F}"/>
-    <hyperlink ref="F71" r:id="rId11" xr:uid="{7A3ECBDB-E535-4B65-A061-9267A9292ADE}"/>
-    <hyperlink ref="F72" r:id="rId12" xr:uid="{AA0EA6C9-359B-4DD4-B29B-31E1B4E72016}"/>
-    <hyperlink ref="F73" r:id="rId13" xr:uid="{D49BC22E-FC53-46B7-A78B-126BD0FA3DB5}"/>
-    <hyperlink ref="F46" r:id="rId14" xr:uid="{12A5BFEB-A875-4840-839C-8B054790EB97}"/>
-    <hyperlink ref="F47" r:id="rId15" xr:uid="{6760ADEB-1ED9-4DF0-93F6-9E1C69CF29FC}"/>
-    <hyperlink ref="F48" r:id="rId16" xr:uid="{7D161BB2-F6E0-4B77-96F3-EA1340168215}"/>
-    <hyperlink ref="F50" r:id="rId17" xr:uid="{32D57917-AE6F-494D-AA32-E441EB6A079F}"/>
-    <hyperlink ref="F51" r:id="rId18" xr:uid="{69F1A799-B95D-4484-B410-26F335B45842}"/>
-    <hyperlink ref="F52" r:id="rId19" xr:uid="{ECFB4D30-9633-4881-B468-D46A967F3460}"/>
-    <hyperlink ref="F55" r:id="rId20" xr:uid="{5CF02266-2A6A-4740-A7F1-D248E7DBD25F}"/>
-    <hyperlink ref="F56" r:id="rId21" xr:uid="{5915C57B-C6AB-49C5-9FA1-9578CF01BFBD}"/>
-    <hyperlink ref="F57" r:id="rId22" xr:uid="{82328BD7-C9CF-4062-A9D1-4A43D38035B4}"/>
-    <hyperlink ref="F59" r:id="rId23" xr:uid="{43405383-4239-4B42-86DE-37B919FC09FB}"/>
-    <hyperlink ref="F60" r:id="rId24" xr:uid="{DE075D6C-8959-49B9-9D77-5C6332B4B8DA}"/>
-    <hyperlink ref="F61" r:id="rId25" xr:uid="{D149283C-ADF8-4B03-BD8B-877C4DC17423}"/>
-    <hyperlink ref="F64" r:id="rId26" xr:uid="{B23B3960-C96D-473E-BF89-5246C651B945}"/>
-    <hyperlink ref="F65" r:id="rId27" xr:uid="{B56C13F6-53AE-447D-A615-AE3C5BAF48F2}"/>
-    <hyperlink ref="F66" r:id="rId28" xr:uid="{1075C6DC-69D3-4549-8457-AE3BF3C4B442}"/>
-    <hyperlink ref="F68" r:id="rId29" xr:uid="{A20A0842-C85C-4F8E-B262-D7FAB59FCEDB}"/>
-    <hyperlink ref="F69" r:id="rId30" xr:uid="{E50DBCBB-6E47-4D79-A306-01F64E6926BA}"/>
-    <hyperlink ref="F41" r:id="rId31" xr:uid="{00C4D5F6-D9C6-4912-9229-CA2E64376E3A}"/>
-    <hyperlink ref="F42" r:id="rId32" xr:uid="{8D784FF9-973D-4416-AE5E-71E72B3070A6}"/>
-    <hyperlink ref="F43" r:id="rId33" xr:uid="{FFBC7B45-33D0-4A1F-9897-3C080883CE06}"/>
+    <hyperlink ref="F34" r:id="rId5" xr:uid="{CE78F98F-7BD2-4EA8-8E67-FCDB77095A12}"/>
+    <hyperlink ref="F35" r:id="rId6" xr:uid="{7DE1F5AC-CC25-429F-A3FC-D507F2EEFB16}"/>
+    <hyperlink ref="F36" r:id="rId7" xr:uid="{E87E436B-A6CF-4293-ACBA-926DFF90FF9C}"/>
+    <hyperlink ref="F38" r:id="rId8" xr:uid="{CD514174-386C-457E-9805-615309DAE21A}"/>
+    <hyperlink ref="F39" r:id="rId9" xr:uid="{01C1FF2F-6262-4AA7-93EE-58639F5D61F0}"/>
+    <hyperlink ref="F40" r:id="rId10" xr:uid="{FB0EA1FA-ADC3-44E4-B571-1621140B470F}"/>
+    <hyperlink ref="F77" r:id="rId11" xr:uid="{7A3ECBDB-E535-4B65-A061-9267A9292ADE}"/>
+    <hyperlink ref="F78" r:id="rId12" xr:uid="{AA0EA6C9-359B-4DD4-B29B-31E1B4E72016}"/>
+    <hyperlink ref="F79" r:id="rId13" xr:uid="{D49BC22E-FC53-46B7-A78B-126BD0FA3DB5}"/>
+    <hyperlink ref="F49" r:id="rId14" xr:uid="{12A5BFEB-A875-4840-839C-8B054790EB97}"/>
+    <hyperlink ref="F50" r:id="rId15" xr:uid="{6760ADEB-1ED9-4DF0-93F6-9E1C69CF29FC}"/>
+    <hyperlink ref="F51" r:id="rId16" xr:uid="{7D161BB2-F6E0-4B77-96F3-EA1340168215}"/>
+    <hyperlink ref="F53" r:id="rId17" xr:uid="{32D57917-AE6F-494D-AA32-E441EB6A079F}"/>
+    <hyperlink ref="F54" r:id="rId18" xr:uid="{69F1A799-B95D-4484-B410-26F335B45842}"/>
+    <hyperlink ref="F55" r:id="rId19" xr:uid="{ECFB4D30-9633-4881-B468-D46A967F3460}"/>
+    <hyperlink ref="F59" r:id="rId20" xr:uid="{5CF02266-2A6A-4740-A7F1-D248E7DBD25F}"/>
+    <hyperlink ref="F60" r:id="rId21" xr:uid="{5915C57B-C6AB-49C5-9FA1-9578CF01BFBD}"/>
+    <hyperlink ref="F61" r:id="rId22" xr:uid="{82328BD7-C9CF-4062-A9D1-4A43D38035B4}"/>
+    <hyperlink ref="F63" r:id="rId23" xr:uid="{43405383-4239-4B42-86DE-37B919FC09FB}"/>
+    <hyperlink ref="F64" r:id="rId24" xr:uid="{DE075D6C-8959-49B9-9D77-5C6332B4B8DA}"/>
+    <hyperlink ref="F65" r:id="rId25" xr:uid="{D149283C-ADF8-4B03-BD8B-877C4DC17423}"/>
+    <hyperlink ref="F69" r:id="rId26" xr:uid="{B23B3960-C96D-473E-BF89-5246C651B945}"/>
+    <hyperlink ref="F70" r:id="rId27" xr:uid="{B56C13F6-53AE-447D-A615-AE3C5BAF48F2}"/>
+    <hyperlink ref="F71" r:id="rId28" xr:uid="{1075C6DC-69D3-4549-8457-AE3BF3C4B442}"/>
+    <hyperlink ref="F73" r:id="rId29" xr:uid="{A20A0842-C85C-4F8E-B262-D7FAB59FCEDB}"/>
+    <hyperlink ref="F74" r:id="rId30" xr:uid="{E50DBCBB-6E47-4D79-A306-01F64E6926BA}"/>
+    <hyperlink ref="F43" r:id="rId31" xr:uid="{00C4D5F6-D9C6-4912-9229-CA2E64376E3A}"/>
+    <hyperlink ref="F44" r:id="rId32" xr:uid="{8D784FF9-973D-4416-AE5E-71E72B3070A6}"/>
+    <hyperlink ref="F45" r:id="rId33" xr:uid="{FFBC7B45-33D0-4A1F-9897-3C080883CE06}"/>
     <hyperlink ref="F8" r:id="rId34" xr:uid="{4D46C10E-C6D4-4B41-8B66-70D5F2FA3BE1}"/>
     <hyperlink ref="F9" r:id="rId35" xr:uid="{BD53E090-37F9-4E13-AF78-B68973469EB5}"/>
     <hyperlink ref="F11" r:id="rId36" xr:uid="{626FDF40-FBEC-469C-8841-8F876E6B0D93}"/>
     <hyperlink ref="F12" r:id="rId37" xr:uid="{2084F117-6494-4417-9FDF-571020A1FF9B}"/>
     <hyperlink ref="F13" r:id="rId38" xr:uid="{A4D43478-BE26-43E3-86DD-A63CC6920DAE}"/>
     <hyperlink ref="F20" r:id="rId39" xr:uid="{8B678113-A157-4982-AA60-FA3944821DE6}"/>
+    <hyperlink ref="F31" r:id="rId40" xr:uid="{90B170F7-4FB5-41EC-9455-B58B9B561480}"/>
+    <hyperlink ref="F56" r:id="rId41" xr:uid="{776C5E15-ACAB-4254-96C3-E812BC4E4E79}"/>
+    <hyperlink ref="F66" r:id="rId42" xr:uid="{92136A75-F441-4C39-8E1A-CAD819084FDB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId43"/>
   <tableParts count="1">
-    <tablePart r:id="rId41"/>
+    <tablePart r:id="rId44"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>